<commit_message>
Task 22, Task 27
</commit_message>
<xml_diff>
--- a/SourceCode/2024/June2024/Pradeepa_Basics/Task 22/Input.xlsx
+++ b/SourceCode/2024/June2024/Pradeepa_Basics/Task 22/Input.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\UiPathIn30Days\SourceCode\2024\June2024\Pradeepa_Basics\Task 22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F888F23D-D597-42C6-9B22-9311DF136432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D063486-01A7-4F42-B00D-86EFE9969DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
     <x:t>smallletters</x:t>
   </x:si>
@@ -38,67 +37,31 @@
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>pradee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ragini</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pradeep</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sarika</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gokul</x:t>
-  </x:si>
-  <x:si>
-    <x:t>surabhi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>buddy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>chinnu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mahesh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>visu</x:t>
+    <x:t>Pradee</x:t>
   </x:si>
   <x:si>
     <x:t>PRADEE</x:t>
   </x:si>
   <x:si>
-    <x:t>RAGINI</x:t>
-  </x:si>
-  <x:si>
     <x:t>success</x:t>
   </x:si>
   <x:si>
-    <x:t>PRADEEP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SARIKA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GOKUL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SURABHI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BUDDY</x:t>
+    <x:t>Chinnu</x:t>
   </x:si>
   <x:si>
     <x:t>CHINNU</x:t>
   </x:si>
   <x:si>
-    <x:t>MAHESH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VISU</x:t>
+    <x:t>Vasu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VASU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mano</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MANO</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -428,10 +391,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C11"/>
+  <x:dimension ref="A1:A5"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C2" sqref="C2"/>
+      <x:selection activeCell="A8" sqref="A8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,50 +418,44 @@
       <x:c r="A2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A5" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A7" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A8" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A9" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-    </x:row>
-    <x:row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A10" s="0" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A11" s="0" t="s">
-        <x:v>12</x:v>
+      <x:c r="C5" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -508,142 +465,4 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:C11"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:3">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3">
-      <x:c r="A5" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3">
-      <x:c r="A6" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3">
-      <x:c r="A7" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3">
-      <x:c r="A8" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:3">
-      <x:c r="A9" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:3">
-      <x:c r="A10" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:3">
-      <x:c r="A11" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
 </file>
</xml_diff>